<commit_message>
Update code, xong connect Database, Update Project Plan/BAR_ProjectPlan_20120113.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Minutes/BAR_MeetingMinutes_20130110.xlsx
+++ b/Documentation/Minutes/BAR_MeetingMinutes_20130110.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="96" windowWidth="22308" windowHeight="9528"/>
+    <workbookView xWindow="380" yWindow="160" windowWidth="16220" windowHeight="9160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Directory" sheetId="2" r:id="rId2"/>
     <sheet name="Task" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
   <si>
     <t>khanhpd60396</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Filter, Sort</t>
-  </si>
-  <si>
     <t>Listing Food</t>
   </si>
   <si>
@@ -283,6 +281,129 @@
   </si>
   <si>
     <t>thanhtm60101</t>
+  </si>
+  <si>
+    <t>.+</t>
+  </si>
+  <si>
+    <t>10/`</t>
+  </si>
+  <si>
+    <t>Connect DB</t>
+  </si>
+  <si>
+    <t>Class DBUtils</t>
+  </si>
+  <si>
+    <t>- Get connection</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>20/01</t>
+  </si>
+  <si>
+    <t>Hoàn thành trang web theo basic</t>
+  </si>
+  <si>
+    <t>Listing nhaa hang</t>
+  </si>
+  <si>
+    <t>Listing mon an</t>
+  </si>
+  <si>
+    <t>List category</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Basic Search</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Search Page</t>
+  </si>
+  <si>
+    <t>Listing</t>
+  </si>
+  <si>
+    <t>Listing Restaurant</t>
+  </si>
+  <si>
+    <t>Id location</t>
+  </si>
+  <si>
+    <t>LIsting</t>
+  </si>
+  <si>
+    <t>delivery de location</t>
+  </si>
+  <si>
+    <t>Listing Menu</t>
+  </si>
+  <si>
+    <t>Id Restaurant</t>
+  </si>
+  <si>
+    <t>Listing menu</t>
+  </si>
+  <si>
+    <t>ko co</t>
+  </si>
+  <si>
+    <t>Id mon</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>- DB to XML</t>
+  </si>
+  <si>
+    <t>AddtoCard</t>
+  </si>
+  <si>
+    <t>Remove From Card</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Update quantity</t>
+  </si>
+  <si>
+    <t>to session</t>
+  </si>
+  <si>
+    <t>Thong Ke</t>
+  </si>
+  <si>
+    <t>Tuan</t>
+  </si>
+  <si>
+    <t>Tu</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>Khanh</t>
   </si>
 </sst>
 </file>
@@ -624,19 +745,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="52.109375" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -653,7 +774,7 @@
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>26</v>
@@ -676,7 +797,7 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -696,10 +817,10 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -707,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -719,10 +840,10 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -730,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -742,10 +863,10 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -765,85 +886,85 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
         <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
         <v>60</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
         <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +980,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -891,14 +1012,14 @@
   <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -962,43 +1083,43 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1009,7 +1130,7 @@
         <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
         <v>31</v>
@@ -1017,14 +1138,14 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1041,7 +1162,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1"/>
       <c r="E22" s="2">
@@ -1050,11 +1171,11 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2">
         <v>41286</v>
@@ -1062,10 +1183,310 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
         <v>82</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>